<commit_message>
add a rename script and rename the leetcode problems
</commit_message>
<xml_diff>
--- a/problem_info.xlsx
+++ b/problem_info.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="11520" windowWidth="24855" windowHeight="12045"/>
+    <workbookView xWindow="240" yWindow="12120" windowWidth="24855" windowHeight="12045"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1194,9 +1194,6 @@
     <t>Pascal's Triangle</t>
   </si>
   <si>
-    <t>Pascal's Triangle II</t>
-  </si>
-  <si>
     <t>Triangle</t>
   </si>
   <si>
@@ -1444,6 +1441,10 @@
   </si>
   <si>
     <t>Integer to Roman</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pascal's Triangle II</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -1752,49 +1753,7 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1808,6 +1767,48 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2120,8 +2121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B176" sqref="B176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2155,39 +2156,39 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="27">
+      <c r="A2" s="30">
         <v>1</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="26">
-        <v>2</v>
-      </c>
-      <c r="D2" s="26">
+      <c r="C2" s="28">
+        <v>2</v>
+      </c>
+      <c r="D2" s="28">
         <v>5</v>
       </c>
-      <c r="E2" s="26" t="s">
-        <v>171</v>
-      </c>
-      <c r="F2" s="26" t="s">
-        <v>173</v>
+      <c r="E2" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
+      <c r="A3" s="31"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
     </row>
     <row r="4" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>8</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C4" s="4">
         <v>2</v>
@@ -2227,7 +2228,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C6" s="4">
         <v>2</v>
@@ -2243,19 +2244,19 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A7" s="29">
+      <c r="A7" s="41">
         <v>21</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="23">
-        <v>2</v>
-      </c>
-      <c r="D7" s="23">
+      <c r="C7" s="40">
+        <v>2</v>
+      </c>
+      <c r="D7" s="40">
         <v>5</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="E7" s="40" t="s">
         <v>16</v>
       </c>
       <c r="F7" s="8" t="s">
@@ -2263,104 +2264,104 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A8" s="24"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
+      <c r="A8" s="36"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
       <c r="F8" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="25"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
+      <c r="A9" s="29"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
       <c r="F9" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A10" s="26">
+      <c r="A10" s="28">
         <v>28</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="26">
-        <v>4</v>
-      </c>
-      <c r="D10" s="26">
+      <c r="C10" s="28">
+        <v>4</v>
+      </c>
+      <c r="D10" s="28">
         <v>5</v>
       </c>
-      <c r="E10" s="26" t="s">
+      <c r="E10" s="28" t="s">
         <v>10</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A11" s="24"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
+      <c r="A11" s="36"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
       <c r="F11" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="25"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
+      <c r="A12" s="29"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
       <c r="F12" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A13" s="27">
+      <c r="A13" s="30">
         <v>50</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="26">
-        <v>3</v>
-      </c>
-      <c r="D13" s="26">
+      <c r="C13" s="28">
+        <v>3</v>
+      </c>
+      <c r="D13" s="28">
         <v>5</v>
       </c>
-      <c r="E13" s="30"/>
+      <c r="E13" s="34"/>
       <c r="F13" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="28"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="31"/>
+      <c r="A14" s="31"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="35"/>
       <c r="F14" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A15" s="27">
+      <c r="A15" s="30">
         <v>56</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="26">
-        <v>4</v>
-      </c>
-      <c r="D15" s="26">
+      <c r="C15" s="28">
+        <v>4</v>
+      </c>
+      <c r="D15" s="28">
         <v>5</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -2371,10 +2372,10 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A16" s="32"/>
-      <c r="B16" s="32"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
+      <c r="A16" s="39"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
       <c r="E16" s="3" t="s">
         <v>24</v>
       </c>
@@ -2383,26 +2384,26 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="28"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
+      <c r="A17" s="31"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
       <c r="E17" s="4" t="s">
         <v>25</v>
       </c>
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A18" s="27">
+      <c r="A18" s="30">
         <v>57</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="26">
-        <v>2</v>
-      </c>
-      <c r="D18" s="26">
+      <c r="C18" s="28">
+        <v>2</v>
+      </c>
+      <c r="D18" s="28">
         <v>5</v>
       </c>
       <c r="E18" s="3" t="s">
@@ -2413,10 +2414,10 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A19" s="32"/>
-      <c r="B19" s="32"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
+      <c r="A19" s="39"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
       <c r="E19" s="3" t="s">
         <v>24</v>
       </c>
@@ -2425,10 +2426,10 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="28"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
+      <c r="A20" s="31"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
       <c r="E20" s="4"/>
       <c r="F20" s="6"/>
     </row>
@@ -2489,19 +2490,19 @@
       <c r="F23" s="7"/>
     </row>
     <row r="24" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A24" s="27">
+      <c r="A24" s="30">
         <v>88</v>
       </c>
-      <c r="B24" s="27" t="s">
+      <c r="B24" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="26">
-        <v>2</v>
-      </c>
-      <c r="D24" s="26">
+      <c r="C24" s="28">
+        <v>2</v>
+      </c>
+      <c r="D24" s="28">
         <v>5</v>
       </c>
-      <c r="E24" s="26" t="s">
+      <c r="E24" s="28" t="s">
         <v>7</v>
       </c>
       <c r="F24" s="3" t="s">
@@ -2509,11 +2510,11 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="25"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
+      <c r="A25" s="29"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
       <c r="F25" s="4" t="s">
         <v>26</v>
       </c>
@@ -2559,19 +2560,19 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A28" s="26">
+      <c r="A28" s="28">
         <v>127</v>
       </c>
-      <c r="B28" s="26" t="s">
+      <c r="B28" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="26">
-        <v>3</v>
-      </c>
-      <c r="D28" s="26">
+      <c r="C28" s="28">
+        <v>3</v>
+      </c>
+      <c r="D28" s="28">
         <v>5</v>
       </c>
-      <c r="E28" s="26" t="s">
+      <c r="E28" s="28" t="s">
         <v>38</v>
       </c>
       <c r="F28" s="3" t="s">
@@ -2579,60 +2580,60 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="25"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
+      <c r="A29" s="29"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
       <c r="F29" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="27">
-        <v>2</v>
-      </c>
-      <c r="B30" s="27" t="s">
+      <c r="A30" s="30">
+        <v>2</v>
+      </c>
+      <c r="B30" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="26">
-        <v>3</v>
-      </c>
-      <c r="D30" s="26">
-        <v>4</v>
-      </c>
-      <c r="E30" s="26" t="s">
+      <c r="C30" s="28">
+        <v>3</v>
+      </c>
+      <c r="D30" s="28">
+        <v>4</v>
+      </c>
+      <c r="E30" s="28" t="s">
         <v>16</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="28"/>
-      <c r="B31" s="28"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
+      <c r="A31" s="31"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
       <c r="F31" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="41" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="39">
+    <row r="32" spans="1:6" s="27" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="25">
         <v>12</v>
       </c>
-      <c r="B32" s="38" t="s">
-        <v>180</v>
-      </c>
-      <c r="C32" s="38">
-        <v>3</v>
-      </c>
-      <c r="D32" s="38">
-        <v>4</v>
-      </c>
-      <c r="E32" s="40"/>
-      <c r="F32" s="38" t="s">
+      <c r="B32" s="24" t="s">
+        <v>179</v>
+      </c>
+      <c r="C32" s="24">
+        <v>3</v>
+      </c>
+      <c r="D32" s="24">
+        <v>4</v>
+      </c>
+      <c r="E32" s="26"/>
+      <c r="F32" s="24" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2675,16 +2676,16 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A35" s="27">
+      <c r="A35" s="30">
         <v>23</v>
       </c>
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="26">
-        <v>3</v>
-      </c>
-      <c r="D35" s="26">
+      <c r="C35" s="28">
+        <v>3</v>
+      </c>
+      <c r="D35" s="28">
         <v>4</v>
       </c>
       <c r="E35" s="3" t="s">
@@ -2695,10 +2696,10 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A36" s="32"/>
-      <c r="B36" s="32"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="24"/>
+      <c r="A36" s="39"/>
+      <c r="B36" s="39"/>
+      <c r="C36" s="36"/>
+      <c r="D36" s="36"/>
       <c r="E36" s="3" t="s">
         <v>45</v>
       </c>
@@ -2707,10 +2708,10 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="28"/>
-      <c r="B37" s="28"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
+      <c r="A37" s="31"/>
+      <c r="B37" s="31"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="29"/>
       <c r="E37" s="6"/>
       <c r="F37" s="4" t="s">
         <v>17</v>
@@ -2775,47 +2776,47 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A41" s="27">
+      <c r="A41" s="30">
         <v>49</v>
       </c>
-      <c r="B41" s="27" t="s">
+      <c r="B41" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="C41" s="26">
-        <v>3</v>
-      </c>
-      <c r="D41" s="26">
+      <c r="C41" s="28">
+        <v>3</v>
+      </c>
+      <c r="D41" s="28">
         <v>4</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F41" s="30"/>
+      <c r="F41" s="34"/>
     </row>
     <row r="42" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="28"/>
-      <c r="B42" s="28"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
+      <c r="A42" s="31"/>
+      <c r="B42" s="31"/>
+      <c r="C42" s="29"/>
+      <c r="D42" s="29"/>
       <c r="E42" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F42" s="31"/>
+      <c r="F42" s="35"/>
     </row>
     <row r="43" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A43" s="27">
+      <c r="A43" s="30">
         <v>67</v>
       </c>
-      <c r="B43" s="27" t="s">
+      <c r="B43" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="C43" s="26">
-        <v>2</v>
-      </c>
-      <c r="D43" s="26">
-        <v>4</v>
-      </c>
-      <c r="E43" s="26" t="s">
+      <c r="C43" s="28">
+        <v>2</v>
+      </c>
+      <c r="D43" s="28">
+        <v>4</v>
+      </c>
+      <c r="E43" s="28" t="s">
         <v>10</v>
       </c>
       <c r="F43" s="3" t="s">
@@ -2823,11 +2824,11 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="28"/>
-      <c r="B44" s="28"/>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25"/>
-      <c r="E44" s="25"/>
+      <c r="A44" s="31"/>
+      <c r="B44" s="31"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="29"/>
+      <c r="E44" s="29"/>
       <c r="F44" s="4" t="s">
         <v>22</v>
       </c>
@@ -2869,19 +2870,19 @@
       </c>
     </row>
     <row r="47" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A47" s="26">
+      <c r="A47" s="28">
         <v>78</v>
       </c>
-      <c r="B47" s="26" t="s">
+      <c r="B47" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="C47" s="26">
-        <v>3</v>
-      </c>
-      <c r="D47" s="26">
-        <v>4</v>
-      </c>
-      <c r="E47" s="26" t="s">
+      <c r="C47" s="28">
+        <v>3</v>
+      </c>
+      <c r="D47" s="28">
+        <v>4</v>
+      </c>
+      <c r="E47" s="28" t="s">
         <v>7</v>
       </c>
       <c r="F47" s="3" t="s">
@@ -2889,11 +2890,11 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="25"/>
-      <c r="B48" s="25"/>
-      <c r="C48" s="25"/>
-      <c r="D48" s="25"/>
-      <c r="E48" s="25"/>
+      <c r="A48" s="29"/>
+      <c r="B48" s="29"/>
+      <c r="C48" s="29"/>
+      <c r="D48" s="29"/>
+      <c r="E48" s="29"/>
       <c r="F48" s="4" t="s">
         <v>58</v>
       </c>
@@ -2919,19 +2920,19 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A50" s="33">
+      <c r="A50" s="32">
         <v>91</v>
       </c>
-      <c r="B50" s="33" t="s">
+      <c r="B50" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="C50" s="26">
-        <v>3</v>
-      </c>
-      <c r="D50" s="26">
-        <v>4</v>
-      </c>
-      <c r="E50" s="26" t="s">
+      <c r="C50" s="28">
+        <v>3</v>
+      </c>
+      <c r="D50" s="28">
+        <v>4</v>
+      </c>
+      <c r="E50" s="28" t="s">
         <v>10</v>
       </c>
       <c r="F50" s="3" t="s">
@@ -2939,11 +2940,11 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="34"/>
-      <c r="B51" s="34"/>
-      <c r="C51" s="25"/>
-      <c r="D51" s="25"/>
-      <c r="E51" s="25"/>
+      <c r="A51" s="33"/>
+      <c r="B51" s="33"/>
+      <c r="C51" s="29"/>
+      <c r="D51" s="29"/>
+      <c r="E51" s="29"/>
       <c r="F51" s="4" t="s">
         <v>61</v>
       </c>
@@ -3013,7 +3014,7 @@
         <v>4</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C55" s="4">
         <v>5</v>
@@ -3047,32 +3048,32 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="68.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A57" s="35">
+      <c r="A57" s="37">
         <v>10</v>
       </c>
-      <c r="B57" s="35" t="s">
+      <c r="B57" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="C57" s="35">
+      <c r="C57" s="37">
         <v>5</v>
       </c>
-      <c r="D57" s="35">
-        <v>3</v>
-      </c>
-      <c r="E57" s="35" t="s">
+      <c r="D57" s="37">
+        <v>3</v>
+      </c>
+      <c r="E57" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="F57" s="36" t="s">
+      <c r="F57" s="23" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="37"/>
-      <c r="B58" s="37"/>
-      <c r="C58" s="37"/>
-      <c r="D58" s="37"/>
-      <c r="E58" s="37"/>
-      <c r="F58" s="38" t="s">
+      <c r="A58" s="38"/>
+      <c r="B58" s="38"/>
+      <c r="C58" s="38"/>
+      <c r="D58" s="38"/>
+      <c r="E58" s="38"/>
+      <c r="F58" s="24" t="s">
         <v>61</v>
       </c>
     </row>
@@ -3137,29 +3138,29 @@
       </c>
     </row>
     <row r="62" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A62" s="26">
+      <c r="A62" s="28">
         <v>29</v>
       </c>
-      <c r="B62" s="26" t="s">
+      <c r="B62" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="C62" s="26">
-        <v>4</v>
-      </c>
-      <c r="D62" s="26">
-        <v>3</v>
-      </c>
-      <c r="E62" s="30"/>
+      <c r="C62" s="28">
+        <v>4</v>
+      </c>
+      <c r="D62" s="28">
+        <v>3</v>
+      </c>
+      <c r="E62" s="34"/>
       <c r="F62" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="25"/>
-      <c r="B63" s="25"/>
-      <c r="C63" s="25"/>
-      <c r="D63" s="25"/>
-      <c r="E63" s="31"/>
+      <c r="A63" s="29"/>
+      <c r="B63" s="29"/>
+      <c r="C63" s="29"/>
+      <c r="D63" s="29"/>
+      <c r="E63" s="35"/>
       <c r="F63" s="4" t="s">
         <v>22</v>
       </c>
@@ -3181,7 +3182,7 @@
         <v>7</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.2">
@@ -3225,19 +3226,19 @@
       </c>
     </row>
     <row r="67" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A67" s="26">
+      <c r="A67" s="28">
         <v>43</v>
       </c>
-      <c r="B67" s="26" t="s">
+      <c r="B67" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="C67" s="26">
-        <v>4</v>
-      </c>
-      <c r="D67" s="26">
-        <v>3</v>
-      </c>
-      <c r="E67" s="26" t="s">
+      <c r="C67" s="28">
+        <v>4</v>
+      </c>
+      <c r="D67" s="28">
+        <v>3</v>
+      </c>
+      <c r="E67" s="28" t="s">
         <v>10</v>
       </c>
       <c r="F67" s="3" t="s">
@@ -3245,29 +3246,29 @@
       </c>
     </row>
     <row r="68" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="25"/>
-      <c r="B68" s="25"/>
-      <c r="C68" s="25"/>
-      <c r="D68" s="25"/>
-      <c r="E68" s="25"/>
+      <c r="A68" s="29"/>
+      <c r="B68" s="29"/>
+      <c r="C68" s="29"/>
+      <c r="D68" s="29"/>
+      <c r="E68" s="29"/>
       <c r="F68" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A69" s="26">
+      <c r="A69" s="28">
         <v>44</v>
       </c>
-      <c r="B69" s="26" t="s">
+      <c r="B69" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="C69" s="26">
+      <c r="C69" s="28">
         <v>5</v>
       </c>
-      <c r="D69" s="26">
-        <v>3</v>
-      </c>
-      <c r="E69" s="26" t="s">
+      <c r="D69" s="28">
+        <v>3</v>
+      </c>
+      <c r="E69" s="28" t="s">
         <v>10</v>
       </c>
       <c r="F69" s="3" t="s">
@@ -3275,21 +3276,21 @@
       </c>
     </row>
     <row r="70" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A70" s="24"/>
-      <c r="B70" s="24"/>
-      <c r="C70" s="24"/>
-      <c r="D70" s="24"/>
-      <c r="E70" s="24"/>
+      <c r="A70" s="36"/>
+      <c r="B70" s="36"/>
+      <c r="C70" s="36"/>
+      <c r="D70" s="36"/>
+      <c r="E70" s="36"/>
       <c r="F70" s="3" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="25"/>
-      <c r="B71" s="25"/>
-      <c r="C71" s="25"/>
-      <c r="D71" s="25"/>
-      <c r="E71" s="25"/>
+      <c r="A71" s="29"/>
+      <c r="B71" s="29"/>
+      <c r="C71" s="29"/>
+      <c r="D71" s="29"/>
+      <c r="E71" s="29"/>
       <c r="F71" s="4" t="s">
         <v>76</v>
       </c>
@@ -3459,7 +3460,7 @@
         <v>81</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C80" s="4">
         <v>5</v>
@@ -3475,19 +3476,19 @@
       </c>
     </row>
     <row r="81" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A81" s="26">
+      <c r="A81" s="28">
         <v>82</v>
       </c>
-      <c r="B81" s="26" t="s">
+      <c r="B81" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="C81" s="26">
-        <v>3</v>
-      </c>
-      <c r="D81" s="26">
-        <v>3</v>
-      </c>
-      <c r="E81" s="26" t="s">
+      <c r="C81" s="28">
+        <v>3</v>
+      </c>
+      <c r="D81" s="28">
+        <v>3</v>
+      </c>
+      <c r="E81" s="28" t="s">
         <v>16</v>
       </c>
       <c r="F81" s="3" t="s">
@@ -3495,11 +3496,11 @@
       </c>
     </row>
     <row r="82" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="25"/>
-      <c r="B82" s="25"/>
-      <c r="C82" s="25"/>
-      <c r="D82" s="25"/>
-      <c r="E82" s="25"/>
+      <c r="A82" s="29"/>
+      <c r="B82" s="29"/>
+      <c r="C82" s="29"/>
+      <c r="D82" s="29"/>
+      <c r="E82" s="29"/>
       <c r="F82" s="4" t="s">
         <v>9</v>
       </c>
@@ -3563,16 +3564,16 @@
       </c>
     </row>
     <row r="86" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A86" s="26">
+      <c r="A86" s="28">
         <v>94</v>
       </c>
-      <c r="B86" s="26" t="s">
+      <c r="B86" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="C86" s="26">
-        <v>4</v>
-      </c>
-      <c r="D86" s="26">
+      <c r="C86" s="28">
+        <v>4</v>
+      </c>
+      <c r="D86" s="28">
         <v>3</v>
       </c>
       <c r="E86" s="3" t="s">
@@ -3583,10 +3584,10 @@
       </c>
     </row>
     <row r="87" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A87" s="24"/>
-      <c r="B87" s="24"/>
-      <c r="C87" s="24"/>
-      <c r="D87" s="24"/>
+      <c r="A87" s="36"/>
+      <c r="B87" s="36"/>
+      <c r="C87" s="36"/>
+      <c r="D87" s="36"/>
       <c r="E87" s="3" t="s">
         <v>51</v>
       </c>
@@ -3595,26 +3596,26 @@
       </c>
     </row>
     <row r="88" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="25"/>
-      <c r="B88" s="25"/>
-      <c r="C88" s="25"/>
-      <c r="D88" s="25"/>
+      <c r="A88" s="29"/>
+      <c r="B88" s="29"/>
+      <c r="C88" s="29"/>
+      <c r="D88" s="29"/>
       <c r="E88" s="6"/>
       <c r="F88" s="4" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="102.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A89" s="27">
+      <c r="A89" s="30">
         <v>103</v>
       </c>
-      <c r="B89" s="27" t="s">
+      <c r="B89" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="C89" s="26">
-        <v>4</v>
-      </c>
-      <c r="D89" s="26">
+      <c r="C89" s="28">
+        <v>4</v>
+      </c>
+      <c r="D89" s="28">
         <v>3</v>
       </c>
       <c r="E89" s="3" t="s">
@@ -3625,10 +3626,10 @@
       </c>
     </row>
     <row r="90" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="28"/>
-      <c r="B90" s="28"/>
-      <c r="C90" s="25"/>
-      <c r="D90" s="25"/>
+      <c r="A90" s="31"/>
+      <c r="B90" s="31"/>
+      <c r="C90" s="29"/>
+      <c r="D90" s="29"/>
       <c r="E90" s="4" t="s">
         <v>93</v>
       </c>
@@ -3637,64 +3638,64 @@
       </c>
     </row>
     <row r="91" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A91" s="26">
+      <c r="A91" s="28">
         <v>105</v>
       </c>
-      <c r="B91" s="26" t="s">
+      <c r="B91" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="C91" s="26">
-        <v>3</v>
-      </c>
-      <c r="D91" s="26">
+      <c r="C91" s="28">
+        <v>3</v>
+      </c>
+      <c r="D91" s="28">
         <v>3</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F91" s="26" t="s">
+      <c r="F91" s="28" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="25"/>
-      <c r="B92" s="25"/>
-      <c r="C92" s="25"/>
-      <c r="D92" s="25"/>
+      <c r="A92" s="29"/>
+      <c r="B92" s="29"/>
+      <c r="C92" s="29"/>
+      <c r="D92" s="29"/>
       <c r="E92" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="F92" s="25"/>
+      <c r="F92" s="29"/>
     </row>
     <row r="93" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A93" s="26">
+      <c r="A93" s="28">
         <v>106</v>
       </c>
-      <c r="B93" s="26" t="s">
+      <c r="B93" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="C93" s="26">
-        <v>3</v>
-      </c>
-      <c r="D93" s="26">
+      <c r="C93" s="28">
+        <v>3</v>
+      </c>
+      <c r="D93" s="28">
         <v>3</v>
       </c>
       <c r="E93" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F93" s="26" t="s">
+      <c r="F93" s="28" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="25"/>
-      <c r="B94" s="25"/>
-      <c r="C94" s="25"/>
-      <c r="D94" s="25"/>
+      <c r="A94" s="29"/>
+      <c r="B94" s="29"/>
+      <c r="C94" s="29"/>
+      <c r="D94" s="29"/>
       <c r="E94" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="F94" s="25"/>
+      <c r="F94" s="29"/>
     </row>
     <row r="95" spans="1:6" ht="35.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A95" s="5">
@@ -3717,19 +3718,19 @@
       </c>
     </row>
     <row r="96" spans="1:6" ht="68.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A96" s="26">
+      <c r="A96" s="28">
         <v>109</v>
       </c>
-      <c r="B96" s="26" t="s">
+      <c r="B96" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="C96" s="26">
-        <v>4</v>
-      </c>
-      <c r="D96" s="26">
-        <v>3</v>
-      </c>
-      <c r="E96" s="26" t="s">
+      <c r="C96" s="28">
+        <v>4</v>
+      </c>
+      <c r="D96" s="28">
+        <v>3</v>
+      </c>
+      <c r="E96" s="28" t="s">
         <v>16</v>
       </c>
       <c r="F96" s="3" t="s">
@@ -3737,11 +3738,11 @@
       </c>
     </row>
     <row r="97" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="25"/>
-      <c r="B97" s="25"/>
-      <c r="C97" s="25"/>
-      <c r="D97" s="25"/>
-      <c r="E97" s="25"/>
+      <c r="A97" s="29"/>
+      <c r="B97" s="29"/>
+      <c r="C97" s="29"/>
+      <c r="D97" s="29"/>
+      <c r="E97" s="29"/>
       <c r="F97" s="4" t="s">
         <v>9</v>
       </c>
@@ -3767,19 +3768,19 @@
       </c>
     </row>
     <row r="99" spans="1:6" ht="68.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A99" s="26">
+      <c r="A99" s="28">
         <v>114</v>
       </c>
-      <c r="B99" s="26" t="s">
+      <c r="B99" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="C99" s="26">
-        <v>3</v>
-      </c>
-      <c r="D99" s="26">
-        <v>3</v>
-      </c>
-      <c r="E99" s="26" t="s">
+      <c r="C99" s="28">
+        <v>3</v>
+      </c>
+      <c r="D99" s="28">
+        <v>3</v>
+      </c>
+      <c r="E99" s="28" t="s">
         <v>34</v>
       </c>
       <c r="F99" s="3" t="s">
@@ -3787,11 +3788,11 @@
       </c>
     </row>
     <row r="100" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="25"/>
-      <c r="B100" s="25"/>
-      <c r="C100" s="25"/>
-      <c r="D100" s="25"/>
-      <c r="E100" s="25"/>
+      <c r="A100" s="29"/>
+      <c r="B100" s="29"/>
+      <c r="C100" s="29"/>
+      <c r="D100" s="29"/>
+      <c r="E100" s="29"/>
       <c r="F100" s="4" t="s">
         <v>94</v>
       </c>
@@ -3835,19 +3836,19 @@
       <c r="F102" s="7"/>
     </row>
     <row r="103" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A103" s="26">
+      <c r="A103" s="28">
         <v>130</v>
       </c>
-      <c r="B103" s="26" t="s">
+      <c r="B103" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="C103" s="26">
-        <v>4</v>
-      </c>
-      <c r="D103" s="26">
-        <v>3</v>
-      </c>
-      <c r="E103" s="26" t="s">
+      <c r="C103" s="28">
+        <v>4</v>
+      </c>
+      <c r="D103" s="28">
+        <v>3</v>
+      </c>
+      <c r="E103" s="28" t="s">
         <v>7</v>
       </c>
       <c r="F103" s="3" t="s">
@@ -3855,11 +3856,11 @@
       </c>
     </row>
     <row r="104" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="25"/>
-      <c r="B104" s="25"/>
-      <c r="C104" s="25"/>
-      <c r="D104" s="25"/>
-      <c r="E104" s="25"/>
+      <c r="A104" s="29"/>
+      <c r="B104" s="29"/>
+      <c r="C104" s="29"/>
+      <c r="D104" s="29"/>
+      <c r="E104" s="29"/>
       <c r="F104" s="4" t="s">
         <v>104</v>
       </c>
@@ -3885,34 +3886,34 @@
       </c>
     </row>
     <row r="106" spans="1:6" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A106" s="26">
-        <v>3</v>
-      </c>
-      <c r="B106" s="26" t="s">
+      <c r="A106" s="28">
+        <v>3</v>
+      </c>
+      <c r="B106" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="C106" s="26">
-        <v>3</v>
-      </c>
-      <c r="D106" s="26">
+      <c r="C106" s="28">
+        <v>3</v>
+      </c>
+      <c r="D106" s="28">
         <v>2</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F106" s="26" t="s">
+      <c r="F106" s="28" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="107" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="25"/>
-      <c r="B107" s="25"/>
-      <c r="C107" s="25"/>
-      <c r="D107" s="25"/>
+      <c r="A107" s="29"/>
+      <c r="B107" s="29"/>
+      <c r="C107" s="29"/>
+      <c r="D107" s="29"/>
       <c r="E107" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F107" s="25"/>
+      <c r="F107" s="29"/>
     </row>
     <row r="108" spans="1:6" ht="35.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A108" s="5">
@@ -3989,19 +3990,19 @@
       <c r="F111" s="7"/>
     </row>
     <row r="112" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A112" s="26">
+      <c r="A112" s="28">
         <v>25</v>
       </c>
-      <c r="B112" s="26" t="s">
+      <c r="B112" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="C112" s="26">
-        <v>4</v>
-      </c>
-      <c r="D112" s="26">
-        <v>2</v>
-      </c>
-      <c r="E112" s="26" t="s">
+      <c r="C112" s="28">
+        <v>4</v>
+      </c>
+      <c r="D112" s="28">
+        <v>2</v>
+      </c>
+      <c r="E112" s="28" t="s">
         <v>16</v>
       </c>
       <c r="F112" s="3" t="s">
@@ -4009,11 +4010,11 @@
       </c>
     </row>
     <row r="113" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="25"/>
-      <c r="B113" s="25"/>
-      <c r="C113" s="25"/>
-      <c r="D113" s="25"/>
-      <c r="E113" s="25"/>
+      <c r="A113" s="29"/>
+      <c r="B113" s="29"/>
+      <c r="C113" s="29"/>
+      <c r="D113" s="29"/>
+      <c r="E113" s="29"/>
       <c r="F113" s="4" t="s">
         <v>9</v>
       </c>
@@ -4155,19 +4156,19 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A121" s="26">
+      <c r="A121" s="28">
         <v>42</v>
       </c>
-      <c r="B121" s="26" t="s">
-        <v>179</v>
-      </c>
-      <c r="C121" s="26">
-        <v>4</v>
-      </c>
-      <c r="D121" s="26">
-        <v>2</v>
-      </c>
-      <c r="E121" s="26" t="s">
+      <c r="B121" s="28" t="s">
+        <v>178</v>
+      </c>
+      <c r="C121" s="28">
+        <v>4</v>
+      </c>
+      <c r="D121" s="28">
+        <v>2</v>
+      </c>
+      <c r="E121" s="28" t="s">
         <v>7</v>
       </c>
       <c r="F121" s="3" t="s">
@@ -4175,11 +4176,11 @@
       </c>
     </row>
     <row r="122" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="25"/>
-      <c r="B122" s="25"/>
-      <c r="C122" s="25"/>
-      <c r="D122" s="25"/>
-      <c r="E122" s="25"/>
+      <c r="A122" s="29"/>
+      <c r="B122" s="29"/>
+      <c r="C122" s="29"/>
+      <c r="D122" s="29"/>
+      <c r="E122" s="29"/>
       <c r="F122" s="4" t="s">
         <v>94</v>
       </c>
@@ -4240,7 +4241,7 @@
       </c>
       <c r="F125" s="7"/>
       <c r="G125" s="19" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="126" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.2">
@@ -4356,19 +4357,19 @@
       <c r="F131" s="7"/>
     </row>
     <row r="132" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A132" s="27">
+      <c r="A132" s="30">
         <v>75</v>
       </c>
-      <c r="B132" s="27" t="s">
+      <c r="B132" s="30" t="s">
         <v>128</v>
       </c>
-      <c r="C132" s="26">
-        <v>4</v>
-      </c>
-      <c r="D132" s="26">
-        <v>2</v>
-      </c>
-      <c r="E132" s="26" t="s">
+      <c r="C132" s="28">
+        <v>4</v>
+      </c>
+      <c r="D132" s="28">
+        <v>2</v>
+      </c>
+      <c r="E132" s="28" t="s">
         <v>7</v>
       </c>
       <c r="F132" s="3" t="s">
@@ -4376,11 +4377,11 @@
       </c>
     </row>
     <row r="133" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A133" s="28"/>
-      <c r="B133" s="28"/>
-      <c r="C133" s="25"/>
-      <c r="D133" s="25"/>
-      <c r="E133" s="25"/>
+      <c r="A133" s="31"/>
+      <c r="B133" s="31"/>
+      <c r="C133" s="29"/>
+      <c r="D133" s="29"/>
+      <c r="E133" s="29"/>
       <c r="F133" s="4" t="s">
         <v>9</v>
       </c>
@@ -4410,7 +4411,7 @@
         <v>80</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C135" s="4">
         <v>2</v>
@@ -4446,19 +4447,19 @@
       </c>
     </row>
     <row r="137" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A137" s="26">
+      <c r="A137" s="28">
         <v>87</v>
       </c>
-      <c r="B137" s="26" t="s">
+      <c r="B137" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="C137" s="26">
+      <c r="C137" s="28">
         <v>5</v>
       </c>
-      <c r="D137" s="26">
-        <v>2</v>
-      </c>
-      <c r="E137" s="26" t="s">
+      <c r="D137" s="28">
+        <v>2</v>
+      </c>
+      <c r="E137" s="28" t="s">
         <v>10</v>
       </c>
       <c r="F137" s="3" t="s">
@@ -4466,11 +4467,11 @@
       </c>
     </row>
     <row r="138" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A138" s="25"/>
-      <c r="B138" s="25"/>
-      <c r="C138" s="25"/>
-      <c r="D138" s="25"/>
-      <c r="E138" s="25"/>
+      <c r="A138" s="29"/>
+      <c r="B138" s="29"/>
+      <c r="C138" s="29"/>
+      <c r="D138" s="29"/>
+      <c r="E138" s="29"/>
       <c r="F138" s="4" t="s">
         <v>61</v>
       </c>
@@ -4494,19 +4495,19 @@
       </c>
     </row>
     <row r="140" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A140" s="26">
+      <c r="A140" s="28">
         <v>90</v>
       </c>
-      <c r="B140" s="26" t="s">
+      <c r="B140" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="C140" s="26">
-        <v>4</v>
-      </c>
-      <c r="D140" s="26">
-        <v>2</v>
-      </c>
-      <c r="E140" s="26" t="s">
+      <c r="C140" s="28">
+        <v>4</v>
+      </c>
+      <c r="D140" s="28">
+        <v>2</v>
+      </c>
+      <c r="E140" s="28" t="s">
         <v>7</v>
       </c>
       <c r="F140" s="3" t="s">
@@ -4514,11 +4515,11 @@
       </c>
     </row>
     <row r="141" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A141" s="25"/>
-      <c r="B141" s="25"/>
-      <c r="C141" s="25"/>
-      <c r="D141" s="25"/>
-      <c r="E141" s="25"/>
+      <c r="A141" s="29"/>
+      <c r="B141" s="29"/>
+      <c r="C141" s="29"/>
+      <c r="D141" s="29"/>
+      <c r="E141" s="29"/>
       <c r="F141" s="4" t="s">
         <v>58</v>
       </c>
@@ -4544,19 +4545,19 @@
       </c>
     </row>
     <row r="143" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A143" s="27">
+      <c r="A143" s="30">
         <v>97</v>
       </c>
-      <c r="B143" s="27" t="s">
+      <c r="B143" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="C143" s="26">
+      <c r="C143" s="28">
         <v>5</v>
       </c>
-      <c r="D143" s="26">
-        <v>2</v>
-      </c>
-      <c r="E143" s="26" t="s">
+      <c r="D143" s="28">
+        <v>2</v>
+      </c>
+      <c r="E143" s="28" t="s">
         <v>10</v>
       </c>
       <c r="F143" s="3" t="s">
@@ -4564,11 +4565,11 @@
       </c>
     </row>
     <row r="144" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A144" s="28"/>
-      <c r="B144" s="28"/>
-      <c r="C144" s="25"/>
-      <c r="D144" s="25"/>
-      <c r="E144" s="25"/>
+      <c r="A144" s="31"/>
+      <c r="B144" s="31"/>
+      <c r="C144" s="29"/>
+      <c r="D144" s="29"/>
+      <c r="E144" s="29"/>
       <c r="F144" s="4" t="s">
         <v>61</v>
       </c>
@@ -4618,7 +4619,7 @@
         <v>110</v>
       </c>
       <c r="B147" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C147" s="4">
         <v>1</v>
@@ -4678,7 +4679,7 @@
         <v>117</v>
       </c>
       <c r="B150" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C150" s="4">
         <v>4</v>
@@ -4828,29 +4829,29 @@
       <c r="F157" s="7"/>
     </row>
     <row r="158" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A158" s="33">
+      <c r="A158" s="32">
         <v>60</v>
       </c>
-      <c r="B158" s="33" t="s">
-        <v>168</v>
-      </c>
-      <c r="C158" s="26">
+      <c r="B158" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="C158" s="28">
         <v>5</v>
       </c>
-      <c r="D158" s="26">
+      <c r="D158" s="28">
         <v>1</v>
       </c>
-      <c r="E158" s="30"/>
+      <c r="E158" s="34"/>
       <c r="F158" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="159" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A159" s="34"/>
-      <c r="B159" s="34"/>
-      <c r="C159" s="25"/>
-      <c r="D159" s="25"/>
-      <c r="E159" s="31"/>
+      <c r="A159" s="33"/>
+      <c r="B159" s="33"/>
+      <c r="C159" s="29"/>
+      <c r="D159" s="29"/>
+      <c r="E159" s="35"/>
       <c r="F159" s="4" t="s">
         <v>22</v>
       </c>
@@ -4876,19 +4877,19 @@
       </c>
     </row>
     <row r="161" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A161" s="26">
+      <c r="A161" s="28">
         <v>85</v>
       </c>
-      <c r="B161" s="26" t="s">
+      <c r="B161" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="C161" s="26">
+      <c r="C161" s="28">
         <v>5</v>
       </c>
-      <c r="D161" s="26">
+      <c r="D161" s="28">
         <v>1</v>
       </c>
-      <c r="E161" s="26" t="s">
+      <c r="E161" s="28" t="s">
         <v>7</v>
       </c>
       <c r="F161" s="3" t="s">
@@ -4896,29 +4897,29 @@
       </c>
     </row>
     <row r="162" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A162" s="25"/>
-      <c r="B162" s="25"/>
-      <c r="C162" s="25"/>
-      <c r="D162" s="25"/>
-      <c r="E162" s="25"/>
+      <c r="A162" s="29"/>
+      <c r="B162" s="29"/>
+      <c r="C162" s="29"/>
+      <c r="D162" s="29"/>
+      <c r="E162" s="29"/>
       <c r="F162" s="4" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="163" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A163" s="26">
+      <c r="A163" s="28">
         <v>95</v>
       </c>
-      <c r="B163" s="26" t="s">
+      <c r="B163" s="28" t="s">
         <v>149</v>
       </c>
-      <c r="C163" s="26">
-        <v>4</v>
-      </c>
-      <c r="D163" s="26">
+      <c r="C163" s="28">
+        <v>4</v>
+      </c>
+      <c r="D163" s="28">
         <v>1</v>
       </c>
-      <c r="E163" s="26" t="s">
+      <c r="E163" s="28" t="s">
         <v>34</v>
       </c>
       <c r="F163" s="3" t="s">
@@ -4926,11 +4927,11 @@
       </c>
     </row>
     <row r="164" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A164" s="25"/>
-      <c r="B164" s="25"/>
-      <c r="C164" s="25"/>
-      <c r="D164" s="25"/>
-      <c r="E164" s="25"/>
+      <c r="A164" s="29"/>
+      <c r="B164" s="29"/>
+      <c r="C164" s="29"/>
+      <c r="D164" s="29"/>
+      <c r="E164" s="29"/>
       <c r="F164" s="4" t="s">
         <v>104</v>
       </c>
@@ -5058,7 +5059,7 @@
         <v>119</v>
       </c>
       <c r="B171" s="4" t="s">
-        <v>156</v>
+        <v>180</v>
       </c>
       <c r="C171" s="4">
         <v>2</v>
@@ -5076,7 +5077,7 @@
         <v>120</v>
       </c>
       <c r="B172" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C172" s="4">
         <v>3</v>
@@ -5096,7 +5097,7 @@
         <v>121</v>
       </c>
       <c r="B173" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C173" s="4">
         <v>2</v>
@@ -5116,7 +5117,7 @@
         <v>122</v>
       </c>
       <c r="B174" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C174" s="4">
         <v>3</v>
@@ -5128,7 +5129,7 @@
         <v>7</v>
       </c>
       <c r="F174" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="175" spans="1:6" ht="35.25" thickBot="1" x14ac:dyDescent="0.2">
@@ -5136,7 +5137,7 @@
         <v>123</v>
       </c>
       <c r="B175" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C175" s="4">
         <v>4</v>
@@ -5156,7 +5157,7 @@
         <v>126</v>
       </c>
       <c r="B176" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C176" s="4">
         <v>4</v>
@@ -5170,6 +5171,158 @@
   </sheetData>
   <autoFilter ref="A1:F176"/>
   <mergeCells count="176">
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="D35:D37"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="E62:E63"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="E67:E68"/>
+    <mergeCell ref="A69:A71"/>
+    <mergeCell ref="B69:B71"/>
+    <mergeCell ref="C69:C71"/>
+    <mergeCell ref="D69:D71"/>
+    <mergeCell ref="E69:E71"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="B81:B82"/>
+    <mergeCell ref="C81:C82"/>
+    <mergeCell ref="D81:D82"/>
+    <mergeCell ref="E81:E82"/>
+    <mergeCell ref="A86:A88"/>
+    <mergeCell ref="B86:B88"/>
+    <mergeCell ref="C86:C88"/>
+    <mergeCell ref="D86:D88"/>
+    <mergeCell ref="F91:F92"/>
+    <mergeCell ref="A93:A94"/>
+    <mergeCell ref="B93:B94"/>
+    <mergeCell ref="C93:C94"/>
+    <mergeCell ref="D93:D94"/>
+    <mergeCell ref="F93:F94"/>
+    <mergeCell ref="A89:A90"/>
+    <mergeCell ref="B89:B90"/>
+    <mergeCell ref="C89:C90"/>
+    <mergeCell ref="D89:D90"/>
+    <mergeCell ref="A91:A92"/>
+    <mergeCell ref="B91:B92"/>
+    <mergeCell ref="C91:C92"/>
+    <mergeCell ref="D91:D92"/>
+    <mergeCell ref="A96:A97"/>
+    <mergeCell ref="B96:B97"/>
+    <mergeCell ref="C96:C97"/>
+    <mergeCell ref="D96:D97"/>
+    <mergeCell ref="E96:E97"/>
+    <mergeCell ref="A99:A100"/>
+    <mergeCell ref="B99:B100"/>
+    <mergeCell ref="C99:C100"/>
+    <mergeCell ref="D99:D100"/>
+    <mergeCell ref="E99:E100"/>
+    <mergeCell ref="F106:F107"/>
+    <mergeCell ref="A112:A113"/>
+    <mergeCell ref="B112:B113"/>
+    <mergeCell ref="C112:C113"/>
+    <mergeCell ref="D112:D113"/>
+    <mergeCell ref="E112:E113"/>
+    <mergeCell ref="A103:A104"/>
+    <mergeCell ref="B103:B104"/>
+    <mergeCell ref="C103:C104"/>
+    <mergeCell ref="D103:D104"/>
+    <mergeCell ref="E103:E104"/>
+    <mergeCell ref="A106:A107"/>
+    <mergeCell ref="B106:B107"/>
+    <mergeCell ref="C106:C107"/>
+    <mergeCell ref="D106:D107"/>
+    <mergeCell ref="D137:D138"/>
+    <mergeCell ref="E137:E138"/>
+    <mergeCell ref="A140:A141"/>
+    <mergeCell ref="B140:B141"/>
+    <mergeCell ref="C140:C141"/>
+    <mergeCell ref="D140:D141"/>
+    <mergeCell ref="E140:E141"/>
+    <mergeCell ref="A121:A122"/>
+    <mergeCell ref="B121:B122"/>
+    <mergeCell ref="C121:C122"/>
+    <mergeCell ref="D121:D122"/>
+    <mergeCell ref="E121:E122"/>
+    <mergeCell ref="A132:A133"/>
+    <mergeCell ref="B132:B133"/>
+    <mergeCell ref="C132:C133"/>
+    <mergeCell ref="D132:D133"/>
+    <mergeCell ref="E132:E133"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="A161:A162"/>
     <mergeCell ref="B161:B162"/>
@@ -5194,158 +5347,6 @@
     <mergeCell ref="A137:A138"/>
     <mergeCell ref="B137:B138"/>
     <mergeCell ref="C137:C138"/>
-    <mergeCell ref="D137:D138"/>
-    <mergeCell ref="E137:E138"/>
-    <mergeCell ref="A140:A141"/>
-    <mergeCell ref="B140:B141"/>
-    <mergeCell ref="C140:C141"/>
-    <mergeCell ref="D140:D141"/>
-    <mergeCell ref="E140:E141"/>
-    <mergeCell ref="A121:A122"/>
-    <mergeCell ref="B121:B122"/>
-    <mergeCell ref="C121:C122"/>
-    <mergeCell ref="D121:D122"/>
-    <mergeCell ref="E121:E122"/>
-    <mergeCell ref="A132:A133"/>
-    <mergeCell ref="B132:B133"/>
-    <mergeCell ref="C132:C133"/>
-    <mergeCell ref="D132:D133"/>
-    <mergeCell ref="E132:E133"/>
-    <mergeCell ref="F106:F107"/>
-    <mergeCell ref="A112:A113"/>
-    <mergeCell ref="B112:B113"/>
-    <mergeCell ref="C112:C113"/>
-    <mergeCell ref="D112:D113"/>
-    <mergeCell ref="E112:E113"/>
-    <mergeCell ref="A103:A104"/>
-    <mergeCell ref="B103:B104"/>
-    <mergeCell ref="C103:C104"/>
-    <mergeCell ref="D103:D104"/>
-    <mergeCell ref="E103:E104"/>
-    <mergeCell ref="A106:A107"/>
-    <mergeCell ref="B106:B107"/>
-    <mergeCell ref="C106:C107"/>
-    <mergeCell ref="D106:D107"/>
-    <mergeCell ref="A96:A97"/>
-    <mergeCell ref="B96:B97"/>
-    <mergeCell ref="C96:C97"/>
-    <mergeCell ref="D96:D97"/>
-    <mergeCell ref="E96:E97"/>
-    <mergeCell ref="A99:A100"/>
-    <mergeCell ref="B99:B100"/>
-    <mergeCell ref="C99:C100"/>
-    <mergeCell ref="D99:D100"/>
-    <mergeCell ref="E99:E100"/>
-    <mergeCell ref="F91:F92"/>
-    <mergeCell ref="A93:A94"/>
-    <mergeCell ref="B93:B94"/>
-    <mergeCell ref="C93:C94"/>
-    <mergeCell ref="D93:D94"/>
-    <mergeCell ref="F93:F94"/>
-    <mergeCell ref="A89:A90"/>
-    <mergeCell ref="B89:B90"/>
-    <mergeCell ref="C89:C90"/>
-    <mergeCell ref="D89:D90"/>
-    <mergeCell ref="A91:A92"/>
-    <mergeCell ref="B91:B92"/>
-    <mergeCell ref="C91:C92"/>
-    <mergeCell ref="D91:D92"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="B81:B82"/>
-    <mergeCell ref="C81:C82"/>
-    <mergeCell ref="D81:D82"/>
-    <mergeCell ref="E81:E82"/>
-    <mergeCell ref="A86:A88"/>
-    <mergeCell ref="B86:B88"/>
-    <mergeCell ref="C86:C88"/>
-    <mergeCell ref="D86:D88"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="E67:E68"/>
-    <mergeCell ref="A69:A71"/>
-    <mergeCell ref="B69:B71"/>
-    <mergeCell ref="C69:C71"/>
-    <mergeCell ref="D69:D71"/>
-    <mergeCell ref="E69:E71"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="E62:E63"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="D35:D37"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E2:E3"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>